<commit_message>
Fix AJE automatic treatment
</commit_message>
<xml_diff>
--- a/tresor-ms/src/test/resources/tests.xlsx
+++ b/tresor-ms/src/test/resources/tests.xlsx
@@ -429,8 +429,8 @@
   </sheetPr>
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.515625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -517,7 +517,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="3" t="n">
-        <v>789012</v>
+        <v>123456</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>

</xml_diff>